<commit_message>
tablas actualizadas y tiempos neuvos para 200 40 1
</commit_message>
<xml_diff>
--- a/TABLAS%20PARA%20EL%20CASO%203/Tablas de casos CON SEGURIDAD.xlsx
+++ b/TABLAS%20PARA%20EL%20CASO%203/Tablas de casos CON SEGURIDAD.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="2" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Esc 3" sheetId="1" r:id="rId1"/>
@@ -6677,34 +6677,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>21.472000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>21.472000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>21.472000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>21.472000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>21.472000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>21.472000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>21.472000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2</c:v>
+                  <c:v>21.472000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2</c:v>
+                  <c:v>21.472000000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2</c:v>
+                  <c:v>21.472000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14838,8 +14838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:K7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -16035,8 +16035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -16224,34 +16224,34 @@
         <v>19</v>
       </c>
       <c r="C8" s="4">
-        <v>2</v>
+        <v>21.472000000000001</v>
       </c>
       <c r="D8" s="4">
-        <v>2</v>
+        <v>21.472000000000001</v>
       </c>
       <c r="E8" s="4">
-        <v>2</v>
+        <v>21.472000000000001</v>
       </c>
       <c r="F8" s="4">
-        <v>2</v>
+        <v>21.472000000000001</v>
       </c>
       <c r="G8" s="4">
-        <v>2</v>
+        <v>21.472000000000001</v>
       </c>
       <c r="H8" s="4">
-        <v>2</v>
+        <v>21.472000000000001</v>
       </c>
       <c r="I8" s="4">
-        <v>2</v>
+        <v>21.472000000000001</v>
       </c>
       <c r="J8" s="4">
-        <v>2</v>
+        <v>21.472000000000001</v>
       </c>
       <c r="K8" s="4">
-        <v>2</v>
+        <v>21.472000000000001</v>
       </c>
       <c r="L8" s="4">
-        <v>2</v>
+        <v>21.472000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
comiitt sin comentarios y tiempos
</commit_message>
<xml_diff>
--- a/TABLAS%20PARA%20EL%20CASO%203/Tablas de casos CON SEGURIDAD.xlsx
+++ b/TABLAS%20PARA%20EL%20CASO%203/Tablas de casos CON SEGURIDAD.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Esc 3" sheetId="1" r:id="rId1"/>
@@ -1685,34 +1685,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>48.122999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>48.122999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>48.122999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>48.122999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>48.122999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>48.122999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>48.122999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6</c:v>
+                  <c:v>48.122999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6</c:v>
+                  <c:v>48.122999999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6</c:v>
+                  <c:v>48.122999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6451,34 +6451,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>48.122999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>48.122999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>48.122999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>48.122999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>48.122999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>48.122999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>48.122999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6</c:v>
+                  <c:v>48.122999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6</c:v>
+                  <c:v>48.122999999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6</c:v>
+                  <c:v>48.122999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14288,8 +14288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H5:I15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -14988,8 +14988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -15175,34 +15175,34 @@
         <v>19</v>
       </c>
       <c r="C8" s="4">
-        <v>6</v>
+        <v>48.122999999999998</v>
       </c>
       <c r="D8" s="4">
-        <v>6</v>
+        <v>48.122999999999998</v>
       </c>
       <c r="E8" s="4">
-        <v>6</v>
+        <v>48.122999999999998</v>
       </c>
       <c r="F8" s="4">
-        <v>6</v>
+        <v>48.122999999999998</v>
       </c>
       <c r="G8" s="4">
-        <v>6</v>
+        <v>48.122999999999998</v>
       </c>
       <c r="H8" s="4">
-        <v>6</v>
+        <v>48.122999999999998</v>
       </c>
       <c r="I8" s="4">
-        <v>6</v>
+        <v>48.122999999999998</v>
       </c>
       <c r="J8" s="4">
-        <v>6</v>
+        <v>48.122999999999998</v>
       </c>
       <c r="K8" s="4">
-        <v>6</v>
+        <v>48.122999999999998</v>
       </c>
       <c r="L8" s="4">
-        <v>6</v>
+        <v>48.122999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>